<commit_message>
EC3: Minor fix to random tests results.
</commit_message>
<xml_diff>
--- a/EC3-C++_Fault_Detection/tests/results/RealScenarioTestResults.xlsx
+++ b/EC3-C++_Fault_Detection/tests/results/RealScenarioTestResults.xlsx
@@ -1471,12 +1471,6 @@
     <xf borderId="31" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="31" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="31" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf borderId="31" fillId="0" fontId="3" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1488,6 +1482,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="31" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="31" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf borderId="32" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -13701,11 +13701,11 @@
         <v>3.0</v>
       </c>
       <c r="E62" s="96" t="str">
-        <f t="shared" ref="E62:E65" si="9">VLOOKUP(B62,$E$27:$H$45,3,FALSE)</f>
+        <f t="shared" ref="E62:E66" si="9">VLOOKUP(B62,$E$27:$H$45,3,FALSE)</f>
         <v>outside_scope</v>
       </c>
       <c r="F62" s="96" t="str">
-        <f t="shared" ref="F62:F65" si="10">VLOOKUP(B62,$E$27:$H$45,4,false)</f>
+        <f t="shared" ref="F62:F66" si="10">VLOOKUP(B62,$E$27:$H$45,4,false)</f>
         <v>no</v>
       </c>
     </row>
@@ -13751,47 +13751,55 @@
       <c r="B65" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="102">
+      <c r="C65" s="98">
         <v>6.0</v>
       </c>
-      <c r="D65" s="103">
+      <c r="D65" s="99">
         <v>1.0</v>
       </c>
-      <c r="E65" s="104" t="str">
+      <c r="E65" s="102" t="str">
         <f t="shared" si="9"/>
         <v>outside_scope</v>
       </c>
-      <c r="F65" s="104" t="str">
+      <c r="F65" s="102" t="str">
         <f t="shared" si="10"/>
         <v>no</v>
       </c>
     </row>
     <row r="66">
-      <c r="B66" s="105" t="s">
+      <c r="B66" s="103" t="s">
         <v>101</v>
       </c>
       <c r="C66" s="49">
         <v>1.0</v>
       </c>
-      <c r="D66" s="106">
+      <c r="D66" s="104">
         <v>2.0</v>
       </c>
-      <c r="E66" s="92"/>
-      <c r="F66" s="92"/>
+      <c r="E66" s="100" t="str">
+        <f t="shared" si="9"/>
+        <v>yes</v>
+      </c>
+      <c r="F66" s="100" t="str">
+        <f t="shared" si="10"/>
+        <v>yes</v>
+      </c>
     </row>
     <row r="67">
-      <c r="B67" s="105" t="s">
+      <c r="B67" s="103" t="s">
         <v>79</v>
       </c>
       <c r="C67" s="49">
         <v>10.0</v>
       </c>
-      <c r="D67" s="106">
+      <c r="D67" s="104">
         <v>1.7</v>
       </c>
+      <c r="E67" s="92"/>
+      <c r="F67" s="92"/>
     </row>
     <row r="68">
-      <c r="B68" s="105"/>
+      <c r="B68" s="103"/>
       <c r="C68" s="49"/>
       <c r="D68" s="49"/>
     </row>
@@ -13803,7 +13811,7 @@
       <c r="D69" s="49"/>
     </row>
     <row r="70">
-      <c r="B70" s="105"/>
+      <c r="B70" s="103"/>
       <c r="C70" s="49"/>
       <c r="D70" s="49"/>
     </row>
@@ -13848,11 +13856,11 @@
       </c>
     </row>
     <row r="75">
-      <c r="E75" s="104" t="str">
+      <c r="E75" s="102" t="str">
         <f t="shared" si="12"/>
         <v>no</v>
       </c>
-      <c r="F75" s="104" t="str">
+      <c r="F75" s="102" t="str">
         <f t="shared" si="13"/>
         <v>yes</v>
       </c>
@@ -13862,22 +13870,22 @@
       <c r="F76" s="92"/>
     </row>
     <row r="77">
-      <c r="B77" s="105"/>
+      <c r="B77" s="103"/>
       <c r="C77" s="49"/>
       <c r="D77" s="49"/>
     </row>
     <row r="78">
-      <c r="B78" s="105"/>
+      <c r="B78" s="103"/>
       <c r="C78" s="49"/>
       <c r="D78" s="49"/>
     </row>
     <row r="79">
-      <c r="B79" s="105"/>
+      <c r="B79" s="103"/>
       <c r="C79" s="49"/>
       <c r="D79" s="49"/>
     </row>
     <row r="80">
-      <c r="B80" s="105"/>
+      <c r="B80" s="103"/>
       <c r="C80" s="49"/>
       <c r="D80" s="49"/>
     </row>

</xml_diff>